<commit_message>
Some changess + rshb with psb
</commit_message>
<xml_diff>
--- a/final_versions/testing.xlsx
+++ b/final_versions/testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="mkb" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="alfa" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="alfa_curr" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="rshb" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="rshb_prem" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="psb" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -399,8 +401,8 @@
   </sheetPr>
   <dimension ref="A2:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -409,11 +411,6 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>МЕГА Онлайн</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>3 мес.</t>
@@ -940,11 +937,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Без опций</t>
-        </is>
-      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>3 мес.</t>
@@ -1281,11 +1273,6 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>С пополнением</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>3 мес.</t>
@@ -1537,11 +1524,6 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>С пополнением и снятием</t>
-        </is>
-      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>3 мес.</t>
@@ -1789,6 +1771,1261 @@
       <c r="F33" t="inlineStr">
         <is>
           <t>4%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:V35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" customWidth="1" min="12" max="12"/>
+    <col width="15.88671875" customWidth="1" min="13" max="13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>«Онлайн-вклад»</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>4 мес.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>18 мес.</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>24 мес.</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>36 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>500000</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.55% </t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Валюта вклада</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Первоначальная сумма вклада</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Максимальная сумма вклада</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>397</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>547</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>1098</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7.2% </t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>От 100 000</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>20 000 000</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>6,55</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>6,55</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>6,55</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>6,55</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>6,55</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>7,15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7.2% </t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>От 1 000 000</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>6,60</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>6,60</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>6,60</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>6,60</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>6,60</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>7,20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3000000</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7.2% </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5000000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7.2% </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>7000000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.6% </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7.2% </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Моя выгода</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1 мес.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3 мес.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4 мес.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>18 мес.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>24 мес.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>36 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>500000</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Валюта вклада</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Сумма вклада</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>367/397</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>547</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>732</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>1098</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>От 10 000</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>От 500 000</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>3000000</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>От 1 500 000</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5000000</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>7000000</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5% </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5.5% </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Вклад «Курс на выгоду»</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Валюта вклада</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Сумма вклада</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>от 30 000</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>6,9%</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Сумма вклада</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Базовая</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>397</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1098</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>от 100 000</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5,80%</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>от 1 000 000</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5,80%</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>от 3 000 000</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5,80%</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>от 10 000 000</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5,80%</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Повышенная</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>от 100 000</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>6,70%</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7,30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>от 1 000 000</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>6,75%</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>6,75%</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>6,75%</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>7,35%</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>от 3 000 000</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>7,40%</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>от 10 000 000</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>6,85%</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>6,85%</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>6,85%</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>7,45%</t>
         </is>
       </c>
     </row>
@@ -1806,7 +3043,7 @@
   <dimension ref="A2:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2046,7 +3283,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2 500 000 ₽</t>
+          <t>50 000 ₽</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2063,7 +3300,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>700 000 ₽</t>
+          <t>2 500 000 ₽</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2080,7 +3317,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>50 000 ₽</t>
+          <t>700 000 ₽</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2392,7 +3629,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A1" sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2625,7 +3862,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:I18"/>
+      <selection activeCell="A19" sqref="A19:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3663,10 +4900,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3839,27 +5076,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4,508 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4,747 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5,476 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5,748 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5,997 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -3871,12 +5108,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4,521 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4,744 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3886,12 +5123,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5,748 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5,997 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -3903,27 +5140,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4,517 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4,748 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5,49 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>5,743 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5,996 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -3935,27 +5172,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4,543 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4,745 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5,495 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5,733 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5,998 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -3967,27 +5204,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4,537 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4,747 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5,485 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5,742 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5,993 %</t>
+          <t>6 %</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -4105,27 +5342,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4,508 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4,747 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5,476 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5,748 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5,997 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -4137,12 +5374,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4,521 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4,744 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4152,12 +5389,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5,748 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>5,997 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -4169,27 +5406,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4,517 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4,748 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5,49 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5,743 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>5,996 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -4201,27 +5438,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4,543 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>4,745 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5,495 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5,733 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>5,998 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -4233,27 +5470,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4,537 %</t>
+          <t>4,5 %</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4,747 %</t>
+          <t>4,75 %</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5,485 %</t>
+          <t>5,5 %</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5,742 %</t>
+          <t>5,75 %</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>5,993 %</t>
+          <t>6 %</t>
         </is>
       </c>
     </row>
@@ -4504,8 +5741,8 @@
   </sheetPr>
   <dimension ref="A2:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -5815,7 +7052,7 @@
   <dimension ref="A2:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -6795,14 +8032,1346 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="A1" sqref="A1:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Вклад «Пополняемый»</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Суммовая группа / Срок вклада</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>91 день</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>92 дня</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>180 дней</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>182 дня</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>270 дней</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>272 дня</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>395 дней</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>540 дней</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>730 дней</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1095 дней</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>от 3 000 до 700 000 вкл.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5,65%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5,65%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5,40%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>5,40%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5,15%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5,15%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>4,80%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>4,40%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>4,10%</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3,60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>от 700 000 до 10 000 000 вкл.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5,75%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5,75%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5,50%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5,50%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5,25%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>5,25%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>4,90%</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4,50%</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>4,20%</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Вклад «Комфортный»</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Суммовая группа / Срок вклада</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>91 день</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>92 дня</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>180 дней</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>182 дня</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>270 дней</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>272 дня</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>395 дней</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>540 дней</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>730 дней</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1095 дней</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>несниж. остаток 10 000</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5,65%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5,65%</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4,65%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4,65%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3,65%</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>3,65%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>3,20%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2,60%</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2,10%</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1,60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>несниж. остаток 700 000</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5,75%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5,75%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4,75%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>4,75%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>3,75%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>3,75%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>3,30%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2,70%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2,20%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1,70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>«Доходный»</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9 мес.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>500000</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>3000000</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5000000</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>10000000</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>20000000</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>6.75%</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:R23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Вклад «Ультра Доходный»</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Суммовая группа / Срок вклада</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3 мес.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>9 мес.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1 год 1 мес.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1,5 года</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2 года</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3 года</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>4 года</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>5 лет</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>от 1,5 до 5 млн</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6,95%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>6,90%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>7,00%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>6,65%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6,35%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>5,95%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>свыше 5 до 10 млн</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6,95%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6,90%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>7,00%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>6,65%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6,35%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>5,95%</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>свыше 10 млн</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6,95%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>6,90%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>6,80%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>7,00%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6,65%</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6,35%</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>5,95%</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Вклад «Ультра Пополняемый»</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Суммовая группа / Срок вклада</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>3 мес.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>9 мес.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1 год 1 мес.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1,5 года</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2 года</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>3 года</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>4 года</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>5 лет</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>от 1,5 до 5 млн</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6,00%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5,75%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5,50%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5,25%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>свыше 5 до 10 млн</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>6,10%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>5,85%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5,60%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5,35%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>свыше 10 млн</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6,20%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>5,95%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5,70%</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>5,45%</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Вклад «Ультра Комфортный»</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Суммовая группа / Срок вклада</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3 мес.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>6 мес.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>9 мес.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1 год 1 мес.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1,5 года</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2 года</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>3 года</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4 года</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>5 лет</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Рубли РФ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>неснижаемый остаток 1,5 млн</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>6,00%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5,00%</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>4,00%</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3,75%</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>неснижаемый остаток 5 млн</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>6,10%</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5,10%</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>4,10%</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3,85%</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>неснижаемый остаток 10 млн</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>6,20%</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>5,20%</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>4,20%</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>3,95%</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0,01%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
We are at the finishing line
</commit_message>
<xml_diff>
--- a/final_versions/testing.xlsx
+++ b/final_versions/testing.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="mkb" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="psb" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -58,9 +59,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -143,44 +144,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -207,15 +208,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -242,7 +242,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -254,142 +253,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -399,1383 +422,316 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:U33"/>
+  <dimension ref="K3:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:U17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="26.5546875" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="inlineStr">
+    <row r="3">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Вклад «МЕГА Онлайн»</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Сумма вклада, в рублях</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>3 мес.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4-5 мес.</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>6 мес.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>9 мес.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1 год</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>7-11 мес.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>13-17 мес.</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
         <is>
           <t>18 мес.</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2 года</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>3 года</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>19-23 мес.</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>24-30 мес.</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>31-36 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>от 1 000 ₽</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>6,5%</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>7%</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>6,8%</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>6,8%</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>6,8%</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Вклад «МЕГА Онлайн»</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+    </row>
+    <row r="6">
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>от 2 000 000 ₽</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>6,5%</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>7%</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>6,8%</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>6,8%</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>6,8%</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+    </row>
+    <row r="8">
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Вклад «МКБ. 30 лет»</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Срок</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>160 дней</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>370 дней</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>540 дней</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Ставка</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>6,9%</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>7,3%</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>7,5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Вклад «Все включено»</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Сумма вклада, в рублях</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>3 мес.</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4-5 мес.</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>6 мес.</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>7-11 мес.</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>12 мес.</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>13-17 мес.</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>18 мес.</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>19-23 мес.</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>24-30 мес.</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>31-36 мес.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>24 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>от 1 000 ₽</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>6,25%</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>6,75%</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>6,5%</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>от 1 000 ₽</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>от 2 000 000 ₽</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>10000000</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Вклад «МКБ. 30 лет»</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>20000000</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>6,8%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Срок</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>160 дней</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>370 дней</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>540 дней</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3 мес.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>6 мес.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1 год</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>18 мес.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2 года</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Ставка</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>6,9%</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>7,3%</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>7,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Вклад «Все включено»</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Сумма вклада, в рублях</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>3 мес.</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>6 мес.</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>12 мес.</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>18 мес.</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>24 мес.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>от 1 000 ₽</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>10000000</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>20000000</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>6,75%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>6,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>3 мес.</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>6 мес.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1 год</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>18 мес.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2 года</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>10000000</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>20000000</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>6,25%</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>4,75%</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>3 мес.</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>6 мес.</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1 год</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>18 мес.</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2 года</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>10000000</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>20000000</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>5,75%</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>4,5%</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1787,16 +743,11 @@
   </sheetPr>
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="16.33203125" customWidth="1" min="12" max="12"/>
-    <col width="15.88671875" customWidth="1" min="13" max="13"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1868,7 +819,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">6.55% </t>
+          <t xml:space="preserve">7.15% </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -2252,7 +1203,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">5.5% </t>
+          <t xml:space="preserve">5% </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -2359,7 +1310,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">5.5% </t>
+          <t xml:space="preserve">5% </t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -2461,7 +1412,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">5.5% </t>
+          <t xml:space="preserve">5% </t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2558,7 +1509,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">5.5% </t>
+          <t xml:space="preserve">5% </t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -3030,7 +1981,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3043,17 +1994,10 @@
   <dimension ref="A2:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="26.88671875" customWidth="1" min="1" max="1"/>
-    <col width="16.33203125" customWidth="1" min="2" max="2"/>
-    <col width="14.5546875" customWidth="1" min="3" max="3"/>
-    <col width="24.21875" customWidth="1" min="4" max="4"/>
-    <col width="25.88671875" customWidth="1" min="5" max="5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3283,7 +2227,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>50 000 ₽</t>
+          <t>700 000 ₽</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3300,7 +2244,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2 500 000 ₽</t>
+          <t>50 000 ₽</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3317,7 +2261,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>700 000 ₽</t>
+          <t>2 500 000 ₽</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3616,7 +2560,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3629,15 +2573,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD11"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="15.109375" customWidth="1" min="1" max="1"/>
-    <col width="20.44140625" customWidth="1" min="2" max="2"/>
-    <col width="28.6640625" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -3849,7 +2788,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3859,26 +2798,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A2:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD28"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Розница</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Премиум</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
@@ -4890,7 +3817,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -4900,17 +3827,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="18.88671875" customWidth="1" min="1" max="1"/>
-    <col width="23.77734375" customWidth="1" min="8" max="8"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -5729,7 +4652,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -5739,17 +4662,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:R25"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A25"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="25.5546875" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Розница</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Премиум</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -6369,7 +5301,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C пополнением</t>
+          <t>С пополнением</t>
         </is>
       </c>
     </row>
@@ -7039,7 +5971,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7052,10 +5984,10 @@
   <dimension ref="A2:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD14"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="B2" t="inlineStr">
@@ -8022,7 +6954,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8035,10 +6967,10 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:N25"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -8687,7 +7619,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8700,10 +7632,10 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:R23"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -9372,6 +8304,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>